<commit_message>
Changes to pull out the plural tags that nest singular elements (param, pubmed_id in IDF and app_param, contact in SDRF) and same for factor value.  Validation and addition filter modified accordingly.
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/gus/GusAppFramework/branches/4.0@13043 4235af6a-31f9-0310-9ad3-ecf6348f2534
</commit_message>
<xml_diff>
--- a/Community/MagetabConverter/Magetab2Xml/samples/test_magetab_appdx9.xlsx
+++ b/Community/MagetabConverter/Magetab2Xml/samples/test_magetab_appdx9.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-7635" yWindow="2415" windowWidth="19440" windowHeight="8085" tabRatio="162" activeTab="1"/>
@@ -10,12 +10,12 @@
     <sheet name="IDF" sheetId="1" r:id="rId1"/>
     <sheet name="SDRF" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="287">
   <si>
     <t>Investigation Title</t>
   </si>
@@ -858,12 +858,30 @@
   </si>
   <si>
     <t>4100000</t>
+  </si>
+  <si>
+    <t>RUM pipeline: alignment and coverage &lt;id=1&gt;</t>
+  </si>
+  <si>
+    <t>RUM pipeline: alignment and coverage &lt;id=2&gt;</t>
+  </si>
+  <si>
+    <t>RUM pipeline: alignment and coverage &lt;id=3&gt;</t>
+  </si>
+  <si>
+    <t>RUM pipeline: alignment and coverage &lt;id=4&gt;</t>
+  </si>
+  <si>
+    <t>RUM pipeline: alignment and coverage &lt;id=5&gt;</t>
+  </si>
+  <si>
+    <t>RUM pipeline: alignment and coverage &lt;id=6&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="41">
     <font>
       <sz val="11"/>
@@ -1519,7 +1537,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1684,8 +1702,7 @@
     <xf numFmtId="49" fontId="8" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="37" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1822,7 +1839,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1857,7 +1873,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2033,7 +2048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IU61"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
@@ -2072,7 +2087,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60">
+    <row r="3" spans="1:10">
       <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
@@ -4160,11 +4175,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DW7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:DV7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1:Z1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="AV7" sqref="AV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4185,33 +4200,33 @@
     <col min="21" max="21" width="22" style="4" customWidth="1"/>
     <col min="22" max="22" width="35.28515625" style="4" customWidth="1"/>
     <col min="23" max="24" width="29.28515625" style="4" customWidth="1"/>
-    <col min="25" max="26" width="49.140625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="37.28515625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="46.5703125" style="4" customWidth="1"/>
-    <col min="29" max="35" width="37.28515625" style="4" customWidth="1"/>
-    <col min="36" max="36" width="30.85546875" style="4" customWidth="1"/>
-    <col min="37" max="37" width="43" style="4" customWidth="1"/>
-    <col min="38" max="38" width="52.28515625" style="4" customWidth="1"/>
-    <col min="39" max="39" width="9.140625" style="30"/>
-    <col min="40" max="40" width="9.140625" style="4"/>
-    <col min="41" max="41" width="36.28515625" style="4" customWidth="1"/>
-    <col min="42" max="42" width="25" style="4" customWidth="1"/>
-    <col min="43" max="47" width="32.5703125" style="4" customWidth="1"/>
-    <col min="48" max="48" width="22.28515625" style="4" customWidth="1"/>
-    <col min="49" max="50" width="36" style="4" customWidth="1"/>
-    <col min="51" max="51" width="21.140625" style="4" customWidth="1"/>
-    <col min="52" max="52" width="39.28515625" style="55" customWidth="1"/>
-    <col min="53" max="53" width="35.7109375" style="55" customWidth="1"/>
-    <col min="54" max="54" width="12.5703125" style="4" customWidth="1"/>
-    <col min="55" max="56" width="71" style="4" customWidth="1"/>
-    <col min="57" max="58" width="27.42578125" style="4" customWidth="1"/>
-    <col min="59" max="61" width="9.140625" style="4"/>
-    <col min="62" max="64" width="20.140625" style="4" customWidth="1"/>
-    <col min="65" max="127" width="9.140625" style="4"/>
-    <col min="128" max="16384" width="9.140625" style="1"/>
+    <col min="25" max="25" width="49.140625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="37.28515625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="46.5703125" style="4" customWidth="1"/>
+    <col min="28" max="34" width="37.28515625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="30.85546875" style="4" customWidth="1"/>
+    <col min="36" max="36" width="43" style="4" customWidth="1"/>
+    <col min="37" max="37" width="52.28515625" style="4" customWidth="1"/>
+    <col min="38" max="38" width="9.140625" style="30"/>
+    <col min="39" max="39" width="9.140625" style="4"/>
+    <col min="40" max="40" width="36.28515625" style="4" customWidth="1"/>
+    <col min="41" max="41" width="25" style="4" customWidth="1"/>
+    <col min="42" max="46" width="32.5703125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="22.28515625" style="4" customWidth="1"/>
+    <col min="48" max="49" width="36" style="4" customWidth="1"/>
+    <col min="50" max="50" width="21.140625" style="4" customWidth="1"/>
+    <col min="51" max="51" width="39.28515625" style="55" customWidth="1"/>
+    <col min="52" max="52" width="35.7109375" style="55" customWidth="1"/>
+    <col min="53" max="53" width="12.5703125" style="4" customWidth="1"/>
+    <col min="54" max="55" width="71" style="4" customWidth="1"/>
+    <col min="56" max="57" width="27.42578125" style="4" customWidth="1"/>
+    <col min="58" max="60" width="9.140625" style="4"/>
+    <col min="61" max="63" width="20.140625" style="4" customWidth="1"/>
+    <col min="64" max="126" width="9.140625" style="4"/>
+    <col min="127" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67">
+    <row r="1" spans="1:66">
       <c r="A1" s="46" t="s">
         <v>28</v>
       </c>
@@ -4287,134 +4302,131 @@
       <c r="Y1" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="59" t="s">
+      <c r="Z1" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="AA1" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB1" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC1" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD1" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE1" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="AF1" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG1" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH1" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="AI1" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK1" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="AA1" s="48" t="s">
-        <v>268</v>
-      </c>
-      <c r="AB1" s="48" t="s">
+      <c r="AL1" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM1" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN1" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="AO1" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR1" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS1" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT1" s="47" t="s">
+        <v>227</v>
+      </c>
+      <c r="AU1" s="46" t="s">
+        <v>265</v>
+      </c>
+      <c r="AV1" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="AD1" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE1" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF1" s="48" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG1" s="48" t="s">
-        <v>90</v>
-      </c>
-      <c r="AH1" s="48" t="s">
-        <v>91</v>
-      </c>
-      <c r="AI1" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="AJ1" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="AK1" s="48" t="s">
+      <c r="AW1" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="AX1" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="BB1" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="BC1" s="51" t="s">
+        <v>240</v>
+      </c>
+      <c r="BD1" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" s="48" t="s">
+      <c r="BE1" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="AM1" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="AN1" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="AO1" s="48" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP1" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="AQ1" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="AR1" s="47" t="s">
-        <v>93</v>
-      </c>
-      <c r="AS1" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="AT1" s="47" t="s">
-        <v>97</v>
-      </c>
-      <c r="AU1" s="47" t="s">
-        <v>227</v>
-      </c>
-      <c r="AV1" s="46" t="s">
-        <v>265</v>
-      </c>
-      <c r="AW1" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="AX1" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="AY1" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="AZ1" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA1" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" s="47" t="s">
+      <c r="BF1" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="BC1" s="51" t="s">
+      <c r="BG1" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="BH1" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="BI1" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="BD1" s="51" t="s">
+      <c r="BJ1" s="51" t="s">
         <v>240</v>
       </c>
-      <c r="BE1" s="52" t="s">
-        <v>32</v>
-      </c>
-      <c r="BF1" s="52" t="s">
-        <v>107</v>
-      </c>
-      <c r="BG1" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="BH1" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="BI1" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="BJ1" s="51" t="s">
-        <v>42</v>
-      </c>
       <c r="BK1" s="51" t="s">
-        <v>240</v>
-      </c>
-      <c r="BL1" s="51" t="s">
         <v>259</v>
       </c>
-      <c r="BM1" s="48" t="s">
+      <c r="BL1" s="48" t="s">
         <v>106</v>
       </c>
+      <c r="BM1" s="46" t="s">
+        <v>262</v>
+      </c>
       <c r="BN1" s="46" t="s">
-        <v>262</v>
-      </c>
-      <c r="BO1" s="46" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:67" ht="15.75">
+    <row r="2" spans="1:66" ht="15.75">
       <c r="A2" s="30" t="s">
         <v>198</v>
       </c>
@@ -4490,132 +4502,129 @@
       <c r="Y2" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="Z2" s="58" t="s">
+      <c r="Z2" s="30">
+        <v>7</v>
+      </c>
+      <c r="AA2" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB2" s="30">
+        <v>155</v>
+      </c>
+      <c r="AC2" s="30">
+        <v>100</v>
+      </c>
+      <c r="AD2" s="30">
+        <v>250</v>
+      </c>
+      <c r="AE2" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF2" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG2" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH2" s="48"/>
+      <c r="AI2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ2" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK2" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="AA2" s="30">
-        <v>7</v>
-      </c>
-      <c r="AB2" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="AC2" s="30">
-        <v>155</v>
-      </c>
-      <c r="AD2" s="30">
+      <c r="AL2" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM2" s="4">
         <v>100</v>
       </c>
-      <c r="AE2" s="30">
-        <v>250</v>
-      </c>
-      <c r="AF2" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG2" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH2" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="AK2" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="AL2" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM2" s="30" t="s">
-        <v>59</v>
-      </c>
       <c r="AN2" s="4">
-        <v>100</v>
-      </c>
-      <c r="AO2" s="4">
         <v>110</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AQ2" s="4">
+      <c r="AP2" s="4">
         <v>63665335</v>
       </c>
+      <c r="AQ2" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="AR2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS2" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AT2" s="4">
+      <c r="AS2" s="4">
         <v>33</v>
       </c>
+      <c r="AT2" s="4" t="s">
+        <v>228</v>
+      </c>
       <c r="AU2" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="AV2" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="AW2" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="AX2" s="33" t="s">
+      <c r="AV2" s="33" t="s">
+        <v>281</v>
+      </c>
+      <c r="AW2" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="AY2" s="54">
+        <v>43177796</v>
+      </c>
       <c r="AZ2" s="54">
-        <v>43177796</v>
-      </c>
-      <c r="BA2" s="54">
         <v>36224414</v>
       </c>
-      <c r="BB2" s="4">
+      <c r="BA2" s="4">
         <v>1.0900000000000001</v>
       </c>
-      <c r="BC2" s="30" t="s">
+      <c r="BB2" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="BD2" s="4" t="s">
+      <c r="BC2" s="4" t="s">
         <v>241</v>
       </c>
+      <c r="BD2" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="BE2" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF2" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="BG2" s="4">
+      <c r="BF2" s="4">
         <v>1.0900000000000001</v>
       </c>
+      <c r="BG2" s="30" t="s">
+        <v>71</v>
+      </c>
       <c r="BH2" s="30" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="BI2" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="BJ2" s="30" t="s">
         <v>219</v>
       </c>
+      <c r="BJ2" s="4" t="s">
+        <v>247</v>
+      </c>
       <c r="BK2" s="4" t="s">
-        <v>247</v>
+        <v>260</v>
       </c>
       <c r="BL2" s="4" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="BM2" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="BN2" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="BO2" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:67" ht="15.75">
+    <row r="3" spans="1:66" ht="15.75">
       <c r="A3" s="30" t="s">
         <v>199</v>
       </c>
@@ -4691,132 +4700,129 @@
       <c r="Y3" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="Z3" s="58" t="s">
+      <c r="Z3" s="30">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB3" s="30">
+        <v>155</v>
+      </c>
+      <c r="AC3" s="30">
+        <v>100</v>
+      </c>
+      <c r="AD3" s="30">
+        <v>250</v>
+      </c>
+      <c r="AE3" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF3" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG3" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH3" s="48"/>
+      <c r="AI3" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AJ3" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="AK3" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="AA3" s="30">
-        <v>10</v>
-      </c>
-      <c r="AB3" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="AC3" s="30">
-        <v>155</v>
-      </c>
-      <c r="AD3" s="30">
+      <c r="AL3" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="AM3" s="4">
         <v>100</v>
       </c>
-      <c r="AE3" s="30">
-        <v>250</v>
-      </c>
-      <c r="AF3" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG3" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH3" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="AK3" s="32" t="s">
-        <v>273</v>
-      </c>
-      <c r="AL3" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM3" s="30" t="s">
-        <v>271</v>
-      </c>
       <c r="AN3" s="4">
-        <v>100</v>
-      </c>
-      <c r="AO3" s="4">
         <v>110</v>
       </c>
-      <c r="AP3" s="4" t="s">
+      <c r="AO3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AQ3" s="4">
+      <c r="AP3" s="4">
         <v>60311687</v>
       </c>
+      <c r="AQ3" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="AR3" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS3" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AT3" s="4">
+      <c r="AS3" s="4">
         <v>33</v>
       </c>
+      <c r="AT3" s="4" t="s">
+        <v>229</v>
+      </c>
       <c r="AU3" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="AV3" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="AW3" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="AX3" s="33" t="s">
+      <c r="AV3" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="AW3" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="AY3" s="4" t="s">
+      <c r="AX3" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="AY3" s="54">
+        <v>48269046</v>
+      </c>
       <c r="AZ3" s="54">
-        <v>48269046</v>
-      </c>
-      <c r="BA3" s="54">
         <v>41998164</v>
       </c>
-      <c r="BB3" s="4">
+      <c r="BA3" s="4">
         <v>1.0900000000000001</v>
       </c>
-      <c r="BC3" s="30" t="s">
+      <c r="BB3" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="BD3" s="4" t="s">
+      <c r="BC3" s="4" t="s">
         <v>242</v>
       </c>
+      <c r="BD3" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="BE3" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF3" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="BG3" s="4">
+      <c r="BF3" s="4">
         <v>1.0900000000000001</v>
       </c>
+      <c r="BG3" s="30" t="s">
+        <v>71</v>
+      </c>
       <c r="BH3" s="30" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="BI3" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="BJ3" s="30" t="s">
         <v>220</v>
       </c>
+      <c r="BJ3" s="4" t="s">
+        <v>248</v>
+      </c>
       <c r="BK3" s="4" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="BL3" s="4" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="BM3" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="BN3" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="BO3" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="4" spans="1:67" ht="15.75">
+    <row r="4" spans="1:66" ht="15.75">
       <c r="A4" s="30" t="s">
         <v>200</v>
       </c>
@@ -4892,132 +4898,129 @@
       <c r="Y4" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="Z4" s="58" t="s">
+      <c r="Z4" s="30">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB4" s="30">
+        <v>155</v>
+      </c>
+      <c r="AC4" s="30">
+        <v>100</v>
+      </c>
+      <c r="AD4" s="30">
+        <v>250</v>
+      </c>
+      <c r="AE4" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF4" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG4" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH4" s="48"/>
+      <c r="AI4" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AJ4" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="AK4" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="AA4" s="30">
-        <v>10</v>
-      </c>
-      <c r="AB4" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="AC4" s="30">
-        <v>155</v>
-      </c>
-      <c r="AD4" s="30">
+      <c r="AL4" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM4" s="4">
         <v>100</v>
       </c>
-      <c r="AE4" s="30">
-        <v>250</v>
-      </c>
-      <c r="AF4" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG4" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH4" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI4" s="48"/>
-      <c r="AJ4" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="AK4" s="32" t="s">
-        <v>274</v>
-      </c>
-      <c r="AL4" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM4" s="30" t="s">
-        <v>59</v>
-      </c>
       <c r="AN4" s="4">
-        <v>100</v>
-      </c>
-      <c r="AO4" s="4">
         <v>110</v>
       </c>
-      <c r="AP4" s="4" t="s">
+      <c r="AO4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AQ4" s="4">
+      <c r="AP4" s="4">
         <v>34874668</v>
       </c>
+      <c r="AQ4" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="AR4" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS4" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AT4" s="4">
+      <c r="AS4" s="4">
         <v>33</v>
       </c>
+      <c r="AT4" s="4" t="s">
+        <v>230</v>
+      </c>
       <c r="AU4" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="AV4" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="AW4" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="AX4" s="33" t="s">
+      <c r="AV4" s="33" t="s">
+        <v>283</v>
+      </c>
+      <c r="AW4" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="AY4" s="4" t="s">
+      <c r="AX4" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="AY4" s="54">
+        <v>17489844</v>
+      </c>
       <c r="AZ4" s="54">
-        <v>17489844</v>
-      </c>
-      <c r="BA4" s="54">
         <v>13874351</v>
       </c>
-      <c r="BB4" s="4">
+      <c r="BA4" s="4">
         <v>1.0900000000000001</v>
       </c>
-      <c r="BC4" s="30" t="s">
+      <c r="BB4" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="BD4" s="4" t="s">
+      <c r="BC4" s="4" t="s">
         <v>243</v>
       </c>
+      <c r="BD4" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="BE4" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF4" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="BG4" s="4">
+      <c r="BF4" s="4">
         <v>1.0900000000000001</v>
       </c>
+      <c r="BG4" s="30" t="s">
+        <v>71</v>
+      </c>
       <c r="BH4" s="30" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="BI4" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="BJ4" s="30" t="s">
         <v>221</v>
       </c>
+      <c r="BJ4" s="4" t="s">
+        <v>249</v>
+      </c>
       <c r="BK4" s="4" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="BL4" s="4" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="BM4" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="BN4" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="BO4" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="5" spans="1:67" ht="15.75">
+    <row r="5" spans="1:66" ht="15.75">
       <c r="A5" s="30" t="s">
         <v>192</v>
       </c>
@@ -5093,134 +5096,131 @@
       <c r="Y5" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="Z5" s="58" t="s">
+      <c r="Z5" s="30">
+        <v>10</v>
+      </c>
+      <c r="AA5" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB5" s="30">
+        <v>155</v>
+      </c>
+      <c r="AC5" s="30">
+        <v>120</v>
+      </c>
+      <c r="AD5" s="30">
+        <v>300</v>
+      </c>
+      <c r="AE5" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF5" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG5" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH5" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ5" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="AK5" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="AA5" s="30">
-        <v>10</v>
-      </c>
-      <c r="AB5" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="AC5" s="30">
-        <v>155</v>
-      </c>
-      <c r="AD5" s="30">
-        <v>120</v>
-      </c>
-      <c r="AE5" s="30">
-        <v>300</v>
-      </c>
-      <c r="AF5" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG5" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH5" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI5" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="AJ5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AK5" s="32" t="s">
-        <v>275</v>
-      </c>
-      <c r="AL5" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM5" s="30" t="s">
+      <c r="AL5" s="30" t="s">
         <v>272</v>
       </c>
+      <c r="AM5" s="4">
+        <v>100</v>
+      </c>
       <c r="AN5" s="4">
-        <v>100</v>
-      </c>
-      <c r="AO5" s="4">
         <v>110</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AO5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AQ5" s="4">
+      <c r="AP5" s="4">
         <v>127083735</v>
       </c>
+      <c r="AQ5" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="AR5" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AT5" s="4">
+      <c r="AS5" s="4">
         <v>33</v>
       </c>
+      <c r="AT5" s="4" t="s">
+        <v>231</v>
+      </c>
       <c r="AU5" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="AV5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AW5" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="AX5" s="33" t="s">
+      <c r="AV5" s="33" t="s">
+        <v>284</v>
+      </c>
+      <c r="AW5" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="AY5" s="4" t="s">
+      <c r="AX5" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="AY5" s="55">
+        <v>102177738</v>
+      </c>
       <c r="AZ5" s="55">
-        <v>102177738</v>
-      </c>
-      <c r="BA5" s="55">
         <v>91873376</v>
       </c>
-      <c r="BB5" s="4">
+      <c r="BA5" s="4">
         <v>1.0900000000000001</v>
       </c>
+      <c r="BB5" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="BC5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="BD5" s="4" t="s">
         <v>244</v>
       </c>
+      <c r="BD5" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="BE5" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF5" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="BG5" s="4">
+      <c r="BF5" s="4">
         <v>1.0900000000000001</v>
       </c>
+      <c r="BG5" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="BH5" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="BI5" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="BJ5" s="4" t="s">
-        <v>76</v>
+        <v>250</v>
       </c>
       <c r="BK5" s="4" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="BL5" s="4" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="BM5" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="BN5" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="BO5" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="6" spans="1:67" ht="15.75">
+    <row r="6" spans="1:66" ht="15.75">
       <c r="A6" s="30" t="s">
         <v>193</v>
       </c>
@@ -5296,134 +5296,131 @@
       <c r="Y6" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="Z6" s="58" t="s">
+      <c r="Z6" s="30">
+        <v>10</v>
+      </c>
+      <c r="AA6" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB6" s="30">
+        <v>155</v>
+      </c>
+      <c r="AC6" s="30">
+        <v>120</v>
+      </c>
+      <c r="AD6" s="30">
+        <v>300</v>
+      </c>
+      <c r="AE6" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF6" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG6" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH6" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ6" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK6" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="AA6" s="30">
-        <v>10</v>
-      </c>
-      <c r="AB6" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="AC6" s="30">
-        <v>155</v>
-      </c>
-      <c r="AD6" s="30">
-        <v>120</v>
-      </c>
-      <c r="AE6" s="30">
-        <v>300</v>
-      </c>
-      <c r="AF6" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG6" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH6" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI6" s="30" t="s">
+      <c r="AL6" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM6" s="4">
         <v>100</v>
       </c>
-      <c r="AJ6" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK6" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="AL6" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM6" s="30" t="s">
-        <v>59</v>
-      </c>
       <c r="AN6" s="4">
-        <v>100</v>
-      </c>
-      <c r="AO6" s="4">
         <v>110</v>
       </c>
-      <c r="AP6" s="4" t="s">
+      <c r="AO6" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AQ6" s="4">
+      <c r="AP6" s="4">
         <v>48315542</v>
       </c>
+      <c r="AQ6" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="AR6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS6" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AT6" s="4">
+      <c r="AS6" s="4">
         <v>33</v>
       </c>
+      <c r="AT6" s="4" t="s">
+        <v>232</v>
+      </c>
       <c r="AU6" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="AV6" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AW6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="AX6" s="33" t="s">
+      <c r="AV6" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="AW6" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="AY6" s="4" t="s">
+      <c r="AX6" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="AY6" s="55">
+        <v>39041207</v>
+      </c>
       <c r="AZ6" s="55">
-        <v>39041207</v>
-      </c>
-      <c r="BA6" s="55">
         <v>35449336</v>
       </c>
-      <c r="BB6" s="4">
+      <c r="BA6" s="4">
         <v>1.0900000000000001</v>
       </c>
+      <c r="BB6" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="BC6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="BD6" s="4" t="s">
         <v>245</v>
       </c>
+      <c r="BD6" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="BE6" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF6" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="BG6" s="4">
+      <c r="BF6" s="4">
         <v>1.0900000000000001</v>
       </c>
+      <c r="BG6" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="BH6" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="BI6" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="BJ6" s="4" t="s">
-        <v>77</v>
+        <v>251</v>
       </c>
       <c r="BK6" s="4" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="BL6" s="4" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="BM6" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="BN6" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="BO6" s="4" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:67" ht="15.75">
+    <row r="7" spans="1:66" ht="15.75">
       <c r="A7" s="30" t="s">
         <v>194</v>
       </c>
@@ -5496,130 +5493,127 @@
       <c r="Y7" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="Z7" s="58" t="s">
+      <c r="Z7" s="30">
+        <v>10</v>
+      </c>
+      <c r="AA7" s="31" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB7" s="30">
+        <v>155</v>
+      </c>
+      <c r="AC7" s="30">
+        <v>120</v>
+      </c>
+      <c r="AD7" s="30">
+        <v>300</v>
+      </c>
+      <c r="AE7" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="AF7" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG7" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH7" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="AI7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ7" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK7" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="AA7" s="30">
-        <v>10</v>
-      </c>
-      <c r="AB7" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="AC7" s="30">
-        <v>155</v>
-      </c>
-      <c r="AD7" s="30">
-        <v>120</v>
-      </c>
-      <c r="AE7" s="30">
-        <v>300</v>
-      </c>
-      <c r="AF7" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="AG7" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH7" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="AI7" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="AJ7" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK7" s="32" t="s">
-        <v>177</v>
-      </c>
-      <c r="AL7" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="AM7" s="30" t="s">
+      <c r="AL7" s="30" t="s">
         <v>59</v>
       </c>
+      <c r="AM7" s="4">
+        <v>100</v>
+      </c>
       <c r="AN7" s="4">
-        <v>100</v>
-      </c>
-      <c r="AO7" s="4">
         <v>110</v>
       </c>
-      <c r="AP7" s="4" t="s">
+      <c r="AO7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AQ7" s="4">
+      <c r="AP7" s="4">
         <v>65466515</v>
       </c>
+      <c r="AQ7" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="AR7" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="AS7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="AT7" s="4">
+      <c r="AS7" s="4">
         <v>33</v>
       </c>
+      <c r="AT7" s="4" t="s">
+        <v>233</v>
+      </c>
       <c r="AU7" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="AV7" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="AW7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="AX7" s="33" t="s">
+      <c r="AV7" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="AW7" s="58" t="s">
         <v>145</v>
       </c>
-      <c r="AY7" s="4" t="s">
+      <c r="AX7" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="AY7" s="55">
+        <v>51393155</v>
+      </c>
       <c r="AZ7" s="55">
-        <v>51393155</v>
-      </c>
-      <c r="BA7" s="55">
         <v>45586727</v>
       </c>
-      <c r="BB7" s="4">
+      <c r="BA7" s="4">
         <v>1.0900000000000001</v>
       </c>
+      <c r="BB7" s="4" t="s">
+        <v>74</v>
+      </c>
       <c r="BC7" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="BD7" s="4" t="s">
         <v>246</v>
       </c>
+      <c r="BD7" s="30" t="s">
+        <v>54</v>
+      </c>
       <c r="BE7" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="BF7" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="BG7" s="4">
+      <c r="BF7" s="4">
         <v>1.0900000000000001</v>
       </c>
+      <c r="BG7" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="BH7" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="BI7" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="BJ7" s="4" t="s">
-        <v>78</v>
+        <v>252</v>
       </c>
       <c r="BK7" s="4" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="BL7" s="4" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="BM7" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="BN7" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="BO7" s="4" t="s">
         <v>257</v>
       </c>
     </row>
@@ -5631,7 +5625,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="1200" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="BO2:BO7 D2:D7" numberStoredAsText="1"/>
+    <ignoredError sqref="BN2:BN7 D2:D7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>